<commit_message>
Nuovi invii e aggiornamento workflowId
Invii eseguiti nuovamente per incoerenza workflowId
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/INVITRO_LIS/1.4/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/INVITRO_LIS/1.4/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE\Validazione\INVITRO_LIS\1.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248BDF68-8D0F-4EC2-8A53-2A281CED5343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F5D6DB-C673-4782-B29D-A7CA89DEFA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4495,73 +4495,73 @@
     <t>subject_application_version: 1.4</t>
   </si>
   <si>
-    <t>2023-09-28T12:36:32Z</t>
-  </si>
-  <si>
-    <t>a5b797c40e9615a8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.8747a285558d13d12dfbd781e1f492608384ca60c4f2930a1c958b8aa8c66126.137120c534^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-09-28T12:38:50Z</t>
-  </si>
-  <si>
-    <t>0f1e988757a122c9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.1c7cbfa5ae563dd3ebf7f5d54b802a5ed30f52ab5cbce7da7abf383ba0dd10f5.d30412ca43^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-09-28T12:39:42Z</t>
-  </si>
-  <si>
-    <t>577d349e0f2554d7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.51604cd705e8137690cd66b5f52ad5a737e73977af63588fa057de72e183b2e6.122ff88eb3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-09-28T12:41:50Z</t>
-  </si>
-  <si>
-    <t>23e90caacc3f583f</t>
-  </si>
-  <si>
-    <t>2023-09-28T12:44:59Z</t>
-  </si>
-  <si>
-    <t>406423f8bceac2cb</t>
-  </si>
-  <si>
-    <t>2023-09-28T12:46:54Z</t>
-  </si>
-  <si>
-    <t>b46e0d1f5b5f44cc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.639ab4a26e26ff8385eb0164019facfbd7628b7581e2fa56ad971551671f7a1a.8997a7baf9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-09-28T12:48:06Z</t>
-  </si>
-  <si>
-    <t>19620bc5bc8d11c1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.e99529bfcfe5c3304bf3441138a9c4c25f3bccd5ae33cd5704b46d04893ba613.21e6d810d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-09-28T12:49:32Z</t>
-  </si>
-  <si>
-    <t>276b913f5d0ea6cc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.56b2ebf62842fced8c9111427cdb3ecbf6fc7fa10cae5a99db6ce8b3f4557d8e.ac9659e498^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>subject_application_id: INVITRO LIS</t>
+  </si>
+  <si>
+    <t>2023-10-02T09:23:22Z</t>
+  </si>
+  <si>
+    <t>8c4b928b389822b5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.8747a285558d13d12dfbd781e1f492608384ca60c4f2930a1c958b8aa8c66126.b1f791842b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-02T09:25:37Z</t>
+  </si>
+  <si>
+    <t>8808754f67c3ce04</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.1c7cbfa5ae563dd3ebf7f5d54b802a5ed30f52ab5cbce7da7abf383ba0dd10f5.d740561f2f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-02T09:29:57Z</t>
+  </si>
+  <si>
+    <t>414db25daecdaa11</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.51604cd705e8137690cd66b5f52ad5a737e73977af63588fa057de72e183b2e6.36a3ca62bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8c9fe9802f84453e</t>
+  </si>
+  <si>
+    <t>2023-10-02T09:32:51Z</t>
+  </si>
+  <si>
+    <t>1981e0c14afbf897</t>
+  </si>
+  <si>
+    <t>2023-10-02T09:34:04Z</t>
+  </si>
+  <si>
+    <t>2023-10-02T09:35:32Z</t>
+  </si>
+  <si>
+    <t>999204b9b13b823d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.639ab4a26e26ff8385eb0164019facfbd7628b7581e2fa56ad971551671f7a1a.97856bd994^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-02T09:36:25Z</t>
+  </si>
+  <si>
+    <t>3f9f1edece47f33b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.e99529bfcfe5c3304bf3441138a9c4c25f3bccd5ae33cd5704b46d04893ba613.9a820abd9b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-02T09:37:32Z</t>
+  </si>
+  <si>
+    <t>352fb9cab197114e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.56b2ebf62842fced8c9111427cdb3ecbf6fc7fa10cae5a99db6ce8b3f4557d8e.f69b4c8f98^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -6500,10 +6500,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="H244" sqref="H244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6570,7 +6570,7 @@
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="54" t="s">
-        <v>863</v>
+        <v>841</v>
       </c>
       <c r="D3" s="46"/>
       <c r="F3" s="12"/>
@@ -12756,16 +12756,16 @@
         <v>406</v>
       </c>
       <c r="F186" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G186" s="24" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="H186" s="24" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="I186" s="24" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="J186" s="25" t="s">
         <v>489</v>
@@ -12802,16 +12802,16 @@
         <v>408</v>
       </c>
       <c r="F187" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G187" s="24" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H187" s="24" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="I187" s="24" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="J187" s="25" t="s">
         <v>489</v>
@@ -12886,16 +12886,16 @@
         <v>412</v>
       </c>
       <c r="F189" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G189" s="24" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="H189" s="24" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="I189" s="24" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J189" s="25" t="s">
         <v>489</v>
@@ -13650,10 +13650,10 @@
         <v>456</v>
       </c>
       <c r="F211" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G211" s="24" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="H211" s="24" t="s">
         <v>851</v>
@@ -13942,10 +13942,10 @@
         <v>472</v>
       </c>
       <c r="F219" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G219" s="24" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="H219" s="24" t="s">
         <v>853</v>
@@ -14234,7 +14234,7 @@
         <v>488</v>
       </c>
       <c r="F227" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G227" s="24"/>
       <c r="H227" s="24"/>
@@ -14572,16 +14572,16 @@
         <v>500</v>
       </c>
       <c r="F236" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G236" s="24" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="H236" s="24" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="I236" s="24" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="J236" s="25" t="s">
         <v>489</v>
@@ -14664,16 +14664,16 @@
         <v>504</v>
       </c>
       <c r="F238" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G238" s="24" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H238" s="24" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="I238" s="24" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="J238" s="25" t="s">
         <v>489</v>
@@ -14870,16 +14870,16 @@
         <v>514</v>
       </c>
       <c r="F243" s="23">
-        <v>45197</v>
+        <v>45201</v>
       </c>
       <c r="G243" s="24" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="H243" s="24" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="I243" s="24" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J243" s="25" t="s">
         <v>489</v>

</xml_diff>

<commit_message>
Ri-esecuzione casi 1-2-4 per disservizio
Ri-esecuzione dei casi 1-2-4 per segnalazione disservizio ed errore "WII_UNKNOWN_LOG", gli altri casi non sono stati ri-eseguiti non essendo richiesti. Aggiornato data.json e check-list
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/INVITRO_LIS/1.4/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/INVITRO_LIS/1.4/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE\Validazione\INVITRO_LIS\1.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F5D6DB-C673-4782-B29D-A7CA89DEFA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A146550-E2CF-4677-B4CF-7946073543DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="585" windowWidth="28515" windowHeight="14175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4498,33 +4498,6 @@
     <t>subject_application_id: INVITRO LIS</t>
   </si>
   <si>
-    <t>2023-10-02T09:23:22Z</t>
-  </si>
-  <si>
-    <t>8c4b928b389822b5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.8747a285558d13d12dfbd781e1f492608384ca60c4f2930a1c958b8aa8c66126.b1f791842b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-02T09:25:37Z</t>
-  </si>
-  <si>
-    <t>8808754f67c3ce04</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.1c7cbfa5ae563dd3ebf7f5d54b802a5ed30f52ab5cbce7da7abf383ba0dd10f5.d740561f2f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-02T09:29:57Z</t>
-  </si>
-  <si>
-    <t>414db25daecdaa11</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.42101.4.4.51604cd705e8137690cd66b5f52ad5a737e73977af63588fa057de72e183b2e6.36a3ca62bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>8c9fe9802f84453e</t>
   </si>
   <si>
@@ -4562,6 +4535,33 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.42101.4.4.56b2ebf62842fced8c9111427cdb3ecbf6fc7fa10cae5a99db6ce8b3f4557d8e.f69b4c8f98^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>224aee9c23fce081</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.8747a285558d13d12dfbd781e1f492608384ca60c4f2930a1c958b8aa8c66126.63a27bb8da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-06T10:06:52Z</t>
+  </si>
+  <si>
+    <t>2023-10-06T10:08:36Z</t>
+  </si>
+  <si>
+    <t>3d7345fdb0399fd0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.1c7cbfa5ae563dd3ebf7f5d54b802a5ed30f52ab5cbce7da7abf383ba0dd10f5.74c6ccee81^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e931b5f2599a65fa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.42101.4.4.51604cd705e8137690cd66b5f52ad5a737e73977af63588fa057de72e183b2e6.1e667df065^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-06T10:09:40Z</t>
   </si>
 </sst>
 </file>
@@ -6503,7 +6503,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H244" sqref="H244"/>
+      <selection pane="bottomRight" activeCell="G189" sqref="G189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -12756,16 +12756,16 @@
         <v>406</v>
       </c>
       <c r="F186" s="23">
-        <v>45201</v>
+        <v>45205</v>
       </c>
       <c r="G186" s="24" t="s">
-        <v>842</v>
+        <v>857</v>
       </c>
       <c r="H186" s="24" t="s">
-        <v>843</v>
+        <v>855</v>
       </c>
       <c r="I186" s="24" t="s">
-        <v>844</v>
+        <v>856</v>
       </c>
       <c r="J186" s="25" t="s">
         <v>489</v>
@@ -12802,16 +12802,16 @@
         <v>408</v>
       </c>
       <c r="F187" s="23">
-        <v>45201</v>
+        <v>45205</v>
       </c>
       <c r="G187" s="24" t="s">
-        <v>845</v>
+        <v>858</v>
       </c>
       <c r="H187" s="24" t="s">
-        <v>846</v>
+        <v>859</v>
       </c>
       <c r="I187" s="24" t="s">
-        <v>847</v>
+        <v>860</v>
       </c>
       <c r="J187" s="25" t="s">
         <v>489</v>
@@ -12886,16 +12886,16 @@
         <v>412</v>
       </c>
       <c r="F189" s="23">
-        <v>45201</v>
+        <v>45205</v>
       </c>
       <c r="G189" s="24" t="s">
-        <v>848</v>
+        <v>863</v>
       </c>
       <c r="H189" s="24" t="s">
-        <v>849</v>
+        <v>861</v>
       </c>
       <c r="I189" s="24" t="s">
-        <v>850</v>
+        <v>862</v>
       </c>
       <c r="J189" s="25" t="s">
         <v>489</v>
@@ -13653,10 +13653,10 @@
         <v>45201</v>
       </c>
       <c r="G211" s="24" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
       <c r="H211" s="24" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
       <c r="I211" s="24" t="s">
         <v>837</v>
@@ -13945,10 +13945,10 @@
         <v>45201</v>
       </c>
       <c r="G219" s="24" t="s">
-        <v>854</v>
+        <v>845</v>
       </c>
       <c r="H219" s="24" t="s">
-        <v>853</v>
+        <v>844</v>
       </c>
       <c r="I219" s="24" t="s">
         <v>837</v>
@@ -14575,13 +14575,13 @@
         <v>45201</v>
       </c>
       <c r="G236" s="24" t="s">
-        <v>855</v>
+        <v>846</v>
       </c>
       <c r="H236" s="24" t="s">
-        <v>856</v>
+        <v>847</v>
       </c>
       <c r="I236" s="24" t="s">
-        <v>857</v>
+        <v>848</v>
       </c>
       <c r="J236" s="25" t="s">
         <v>489</v>
@@ -14667,13 +14667,13 @@
         <v>45201</v>
       </c>
       <c r="G238" s="24" t="s">
-        <v>858</v>
+        <v>849</v>
       </c>
       <c r="H238" s="24" t="s">
-        <v>859</v>
+        <v>850</v>
       </c>
       <c r="I238" s="24" t="s">
-        <v>860</v>
+        <v>851</v>
       </c>
       <c r="J238" s="25" t="s">
         <v>489</v>
@@ -14873,13 +14873,13 @@
         <v>45201</v>
       </c>
       <c r="G243" s="24" t="s">
-        <v>861</v>
+        <v>852</v>
       </c>
       <c r="H243" s="24" t="s">
-        <v>862</v>
+        <v>853</v>
       </c>
       <c r="I243" s="24" t="s">
-        <v>863</v>
+        <v>854</v>
       </c>
       <c r="J243" s="25" t="s">
         <v>489</v>

</xml_diff>